<commit_message>
finish use cases fot the last paragraph
</commit_message>
<xml_diff>
--- a/tests/ahdab/requestMonthlyReport.xlsx
+++ b/tests/ahdab/requestMonthlyReport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\labRep\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\labRep\tests\ahdab\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t xml:space="preserve">Use Case: </t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>Manager ID</t>
   </si>
   <si>
     <t>Status</t>
@@ -101,93 +98,74 @@
     <t>CompleteRequestion</t>
   </si>
   <si>
-    <t>incorrectID</t>
-  </si>
-  <si>
-    <t>Open "monthly Report"
-Type Manager's ID: "65432198"
-Type Date : "1/3/2016 - 30/3/2016"
-Press : "Send Request"</t>
-  </si>
-  <si>
-    <t>Id must be 9 digits</t>
-  </si>
-  <si>
-    <t>System shows "illegible ID" Error message</t>
-  </si>
-  <si>
-    <t>ManagerNotFound</t>
-  </si>
-  <si>
-    <t>system shows "incorrect ID" Error message</t>
-  </si>
-  <si>
-    <t>failed to approve Manager's id</t>
-  </si>
-  <si>
-    <t>MissingManagerID</t>
-  </si>
-  <si>
-    <t>Open "monthly Report"
-Type Manager's ID: ""
-Type Date : ""
-Press : "Send Request"</t>
-  </si>
-  <si>
-    <t>System shows "Enter ID" message</t>
-  </si>
-  <si>
     <t>CancelRequestion</t>
   </si>
   <si>
+    <t>System ask "are you sure of canceling the requestion"</t>
+  </si>
+  <si>
+    <t>incorrestDtaeDomain</t>
+  </si>
+  <si>
+    <t>System throws "illegible Date Doman" Error message</t>
+  </si>
+  <si>
+    <t>Domain Dates most
+ be one month 
+-30 days</t>
+  </si>
+  <si>
+    <t>SendingFailed</t>
+  </si>
+  <si>
+    <t>System throws "sending th request failed, try again later" message</t>
+  </si>
+  <si>
+    <t>No Internet 
+connection</t>
+  </si>
+  <si>
+    <t>Report Date</t>
+  </si>
+  <si>
+    <t>yes-Report exists in the DB
+no-Report not exists in the DB</t>
+  </si>
+  <si>
+    <t>Reports that  in the system</t>
+  </si>
+  <si>
+    <t>1/3/2016 - 30/3/2016</t>
+  </si>
+  <si>
     <t xml:space="preserve">Open "monthly Report"
-Type Manager's ID: "456123789"
 Type Date : "1/3/2016 - 30/3/2016"
 press : "Cancel"
 </t>
   </si>
   <si>
-    <t>System ask "are you sure of canceling the requestion"</t>
-  </si>
-  <si>
-    <t>incorrestDtaeDomain</t>
-  </si>
-  <si>
     <t>Open "monthly Report"
-Type Manager's ID: "456123789"
 Type Date : "1/3/2016 - 5/4/2016"
 Press : "Send Request"</t>
   </si>
   <si>
-    <t>System throws "illegible Date Doman" Error message</t>
-  </si>
-  <si>
-    <t>Domain Dates most
- be one month 
--30 days</t>
-  </si>
-  <si>
-    <t>SendingFailed</t>
-  </si>
-  <si>
     <t>Open "monthly Report"
-Type Manager's ID: "456123789"
-Type Date : "1/3/2016 - 30/6/2016"
+Type Date : "1/3/2016 - 30/3/2016"
 Press : "Send Request"</t>
   </si>
   <si>
-    <t>System throws "sending th request failed, try again later" message</t>
-  </si>
-  <si>
-    <t>No Internet 
-connection</t>
-  </si>
-  <si>
-    <t>Managers that have account in the system</t>
-  </si>
-  <si>
-    <t>yes-manager exists in the DB
-no-manager not exists in the DB</t>
+    <t>Open "monthly Report"
+Type Date : ""
+Press : "Send Request"</t>
+  </si>
+  <si>
+    <t>System shows "Enter Date" message</t>
+  </si>
+  <si>
+    <t>MissingDate</t>
+  </si>
+  <si>
+    <t>1/4/2016 - 30/4/2016</t>
   </si>
 </sst>
 </file>
@@ -547,6 +525,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -561,12 +545,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -850,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -864,17 +842,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="20"/>
+      <c r="A1" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -882,7 +860,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -895,7 +873,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="19"/>
     </row>
@@ -907,61 +885,57 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>12</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="8">
-        <v>456123789</v>
+      <c r="A9" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="10"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="8">
-        <v>65432198</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="C10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A11" s="11">
-        <v>654321987</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="13"/>
     </row>
     <row r="12" spans="1:7" ht="57.75" customHeight="1" thickBot="1">
-      <c r="A12" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
+      <c r="A12" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="25"/>
     </row>
     <row r="14" spans="1:7" ht="18.75">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="14" t="s">
@@ -979,98 +953,82 @@
     </row>
     <row r="16" spans="1:7" ht="60">
       <c r="A16" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="18"/>
+    </row>
+    <row r="19" spans="1:4" ht="45">
+      <c r="A19" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="60">
+      <c r="A20" s="20" t="s">
         <v>22</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="60">
-      <c r="A17" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="60">
-      <c r="A18" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="60">
-      <c r="A19" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="75">
-      <c r="A20" s="25" t="s">
-        <v>33</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="60">
+      <c r="A21" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="19" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="60">
-      <c r="A21" s="25" t="s">
+      <c r="C21" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="75">
+      <c r="A22" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="75">
-      <c r="A22" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>42</v>
+      <c r="C22" s="21" t="s">
+        <v>28</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="25"/>
+      <c r="A23" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>